<commit_message>
- helper method to detect boxed context with result and its test - test to generate the context string for boxed context with result
</commit_message>
<xml_diff>
--- a/test/data/RoutingDecisionService.xlsx
+++ b/test/data/RoutingDecisionService.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7020" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Routing" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="115">
   <si>
     <t>service</t>
   </si>
@@ -383,6 +383,9 @@
   </si>
   <si>
     <t>"SELF-EMPLOYED"</t>
+  </si>
+  <si>
+    <t>context-with-result</t>
   </si>
 </sst>
 </file>
@@ -432,7 +435,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -498,28 +501,6 @@
       </left>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -529,62 +510,55 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -868,69 +842,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27" customWidth="1"/>
-    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="13"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="3"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="3"/>
+      <c r="D7" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -945,55 +919,64 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:C6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="24.85546875" customWidth="1"/>
     <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="19"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="14"/>
-    </row>
-    <row r="4" spans="2:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="23" t="s">
         <v>86</v>
       </c>
+      <c r="D4" s="23"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="17" t="s">
         <v>88</v>
       </c>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B3:C3"/>
+  <mergeCells count="4">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="B6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1003,7 +986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1018,44 +1001,44 @@
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1072,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1091,234 +1074,234 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="3">
+      <c r="D6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2">
         <v>32</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="3">
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="3">
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="D10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2">
         <v>48</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>6</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="3">
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>7</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="3">
+      <c r="E12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="2">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>8</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="2">
         <v>15</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>9</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="2">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>10</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="2">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>11</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E16" s="3" t="s">
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="2">
         <v>36</v>
       </c>
     </row>
@@ -1331,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1346,163 +1329,163 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="19"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="9"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="15" t="s">
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>1</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="3" t="b">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G6" s="3" t="s">
+      <c r="E6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="3" t="b">
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="D8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="B9" s="2">
+        <v>4</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G10" s="3" t="s">
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1515,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,44 +1512,44 @@
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="C4" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="16"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="16"/>
+      <c r="D6" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1583,8 +1566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,219 +1584,219 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="23" t="b">
+      <c r="C5" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="3" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
-        <v>4</v>
-      </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23" t="s">
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>5</v>
       </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="3" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>6</v>
       </c>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="3" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="F10" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>7</v>
       </c>
-      <c r="C11" s="23"/>
-      <c r="D11" s="24" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>8</v>
       </c>
-      <c r="C12" s="23" t="b">
+      <c r="C12" s="18" t="b">
         <v>1</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>9</v>
       </c>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
+      <c r="B14" s="2">
         <v>10</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
+      <c r="B15" s="2">
         <v>11</v>
       </c>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23" t="s">
+      <c r="C15" s="18"/>
+      <c r="D15" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="3">
+      <c r="B16" s="2">
         <v>12</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="3" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="3">
+      <c r="B17" s="2">
         <v>13</v>
       </c>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="3" t="s">
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1834,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1848,71 +1831,71 @@
       <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="16"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="13"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="13"/>
+      <c r="D6" s="16"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="16"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="D8" s="13"/>
+      <c r="D8" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1920,63 +1903,76 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C7"/>
+  <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="26"/>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
+      <c r="D4" s="17"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="6" spans="2:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D5" s="17"/>
+    </row>
+    <row r="6" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="23" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="21"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B7:C7"/>
+  <mergeCells count="5">
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B7:D7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1987,7 +1983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2002,26 +1998,26 @@
       <c r="B2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="10"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="13"/>
+      <c r="D4" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2036,8 +2032,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,57 +2049,57 @@
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>0.6</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="2">
         <v>0.7</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>0.8</v>
       </c>
     </row>
@@ -2116,81 +2112,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C1" s="19"/>
+      <c r="C1" s="8"/>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="19"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="19"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="27"/>
-      <c r="E6" s="19"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="19"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="D8" s="19"/>
+      <c r="D8" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B3:C3"/>
+  <mergeCells count="5">
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
- fixed typo in the excel workbook (test data); double quotes issue - impl for parsing boxed context with result
</commit_message>
<xml_diff>
--- a/test/data/RoutingDecisionService.xlsx
+++ b/test/data/RoutingDecisionService.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Routing" sheetId="1" r:id="rId1"/>
@@ -297,95 +297,95 @@
     <t>Monthly Fee</t>
   </si>
   <si>
-    <t>if Product Type = “STANDARD LOAN”
+    <t>Monthly Repayment</t>
+  </si>
+  <si>
+    <t>PMT (Rate, Term, Amount)</t>
+  </si>
+  <si>
+    <t>Monthly Repayment + Monthly Fee</t>
+  </si>
+  <si>
+    <t>Application risk score model</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Applicant data . Age</t>
+  </si>
+  <si>
+    <t>Marital Status</t>
+  </si>
+  <si>
+    <t>Applicant data . MaritalStatus</t>
+  </si>
+  <si>
+    <t>Employment Status</t>
+  </si>
+  <si>
+    <t>Applicant data . EmploymentStatus</t>
+  </si>
+  <si>
+    <t>Application Risk Score Model</t>
+  </si>
+  <si>
+    <t>C+</t>
+  </si>
+  <si>
+    <t>Partial Score</t>
+  </si>
+  <si>
+    <t>[18..120]</t>
+  </si>
+  <si>
+    <t>"S", "M"</t>
+  </si>
+  <si>
+    <t>"UNEMPLOYED", "EMPLOYED", "SELF-EMPLOYED", "STUDENT"</t>
+  </si>
+  <si>
+    <t>[18..21]</t>
+  </si>
+  <si>
+    <t>[22..25]</t>
+  </si>
+  <si>
+    <t>[26..35]</t>
+  </si>
+  <si>
+    <t>[36..49]</t>
+  </si>
+  <si>
+    <t>&gt;=50</t>
+  </si>
+  <si>
+    <t>"S"</t>
+  </si>
+  <si>
+    <t>"M"</t>
+  </si>
+  <si>
+    <t>"UNEMPLOYED"</t>
+  </si>
+  <si>
+    <t>"STUDENT"</t>
+  </si>
+  <si>
+    <t>"EMPLOYED"</t>
+  </si>
+  <si>
+    <t>"SELF-EMPLOYED"</t>
+  </si>
+  <si>
+    <t>context-with-result</t>
+  </si>
+  <si>
+    <t>if Product Type = "STANDARD LOAN"
 then 20.00
-else if Product Type = “SPECIAL LOAN”
+else if Product Type = "SPECIAL LOAN"
 then 25.00
 else null</t>
-  </si>
-  <si>
-    <t>Monthly Repayment</t>
-  </si>
-  <si>
-    <t>PMT (Rate, Term, Amount)</t>
-  </si>
-  <si>
-    <t>Monthly Repayment + Monthly Fee</t>
-  </si>
-  <si>
-    <t>Application risk score model</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Applicant data . Age</t>
-  </si>
-  <si>
-    <t>Marital Status</t>
-  </si>
-  <si>
-    <t>Applicant data . MaritalStatus</t>
-  </si>
-  <si>
-    <t>Employment Status</t>
-  </si>
-  <si>
-    <t>Applicant data . EmploymentStatus</t>
-  </si>
-  <si>
-    <t>Application Risk Score Model</t>
-  </si>
-  <si>
-    <t>C+</t>
-  </si>
-  <si>
-    <t>Partial Score</t>
-  </si>
-  <si>
-    <t>[18..120]</t>
-  </si>
-  <si>
-    <t>"S", "M"</t>
-  </si>
-  <si>
-    <t>"UNEMPLOYED", "EMPLOYED", "SELF-EMPLOYED", "STUDENT"</t>
-  </si>
-  <si>
-    <t>[18..21]</t>
-  </si>
-  <si>
-    <t>[22..25]</t>
-  </si>
-  <si>
-    <t>[26..35]</t>
-  </si>
-  <si>
-    <t>[36..49]</t>
-  </si>
-  <si>
-    <t>&gt;=50</t>
-  </si>
-  <si>
-    <t>"S"</t>
-  </si>
-  <si>
-    <t>"M"</t>
-  </si>
-  <si>
-    <t>"UNEMPLOYED"</t>
-  </si>
-  <si>
-    <t>"STUDENT"</t>
-  </si>
-  <si>
-    <t>"EMPLOYED"</t>
-  </si>
-  <si>
-    <t>"SELF-EMPLOYED"</t>
-  </si>
-  <si>
-    <t>context-with-result</t>
   </si>
 </sst>
 </file>
@@ -552,13 +552,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -842,7 +842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,37 +936,37 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
     </row>
     <row r="4" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>85</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>86</v>
+        <v>114</v>
       </c>
       <c r="D4" s="23"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>88</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -1008,35 +1008,35 @@
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>91</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>92</v>
       </c>
       <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>95</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>96</v>
       </c>
       <c r="D6" s="17"/>
     </row>
@@ -1070,7 +1070,7 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -1092,31 +1092,31 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>102</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1125,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
@@ -1142,14 +1142,14 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1157,7 +1157,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
@@ -1174,7 +1174,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>4</v>
@@ -1191,7 +1191,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
@@ -1211,7 +1211,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>4</v>
@@ -1228,7 +1228,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>4</v>
@@ -1248,7 +1248,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F13" s="2">
         <v>15</v>
@@ -1265,7 +1265,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F14" s="2">
         <v>18</v>
@@ -1282,7 +1282,7 @@
         <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F15" s="2">
         <v>45</v>
@@ -1299,7 +1299,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F16" s="2">
         <v>36</v>
@@ -1922,15 +1922,15 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">

</xml_diff>

<commit_message>
test cases to test if the workbook is incorrect format
</commit_message>
<xml_diff>
--- a/test/data/RoutingDecisionService.xlsx
+++ b/test/data/RoutingDecisionService.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Routing" sheetId="1" r:id="rId1"/>
@@ -919,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- added a json-feel object for the routing decision service (test data) - changed logic to pass the pegjs parsing tests - edited the excel test data for correctness
</commit_message>
<xml_diff>
--- a/test/data/RoutingDecisionService.xlsx
+++ b/test/data/RoutingDecisionService.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670" firstSheet="7" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Routing" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="113">
   <si>
     <t>service</t>
   </si>
@@ -73,24 +73,12 @@
     <t>Bureau data . Credit Score</t>
   </si>
   <si>
-    <t>Post-bureau risk category</t>
-  </si>
-  <si>
-    <t>Post-Bureau Affordability</t>
-  </si>
-  <si>
-    <t>Post-bureau affordability</t>
-  </si>
-  <si>
     <t>invocation</t>
   </si>
   <si>
     <t>P</t>
   </si>
   <si>
-    <t>Post-Bureau Risk Category</t>
-  </si>
-  <si>
     <t>"HIGH"</t>
   </si>
   <si>
@@ -109,12 +97,6 @@
     <t>"DECLINE", "REFER", "ACCEPT"</t>
   </si>
   <si>
-    <t>Post-Bureau risk category</t>
-  </si>
-  <si>
-    <t>Post-Bureau risk category table</t>
-  </si>
-  <si>
     <t>Existing Customer</t>
   </si>
   <si>
@@ -130,9 +112,6 @@
     <t>Application risk score</t>
   </si>
   <si>
-    <t>Post-bureau risk category table</t>
-  </si>
-  <si>
     <t>&lt; 120</t>
   </si>
   <si>
@@ -238,9 +217,6 @@
     <t>Credit Contingency Factor</t>
   </si>
   <si>
-    <t>Credit-contingency-factor</t>
-  </si>
-  <si>
     <t>Affordability</t>
   </si>
   <si>
@@ -319,9 +295,6 @@
     <t>Applicant data . EmploymentStatus</t>
   </si>
   <si>
-    <t>Application Risk Score Model</t>
-  </si>
-  <si>
     <t>C+</t>
   </si>
   <si>
@@ -373,14 +346,34 @@
     <t>context-with-result</t>
   </si>
   <si>
-    <t>if Product Type = "STANDARD LOAN"
-then 20.00
-else if Product Type = "SPECIAL LOAN"
-then 25.00
-else null</t>
-  </si>
-  <si>
     <t>if Disposable Income * Credit Contingency Factor &gt; Required Monthly Installment then true else false</t>
+  </si>
+  <si>
+    <t>Credit contingency factor</t>
+  </si>
+  <si>
+    <t>Post bureau risk category</t>
+  </si>
+  <si>
+    <t>Post bureau affordability</t>
+  </si>
+  <si>
+    <t>Post Bureau Risk Category</t>
+  </si>
+  <si>
+    <t>Post Bureau Affordability</t>
+  </si>
+  <si>
+    <t>Post Bureau risk category</t>
+  </si>
+  <si>
+    <t>Post Bureau risk category table</t>
+  </si>
+  <si>
+    <t>Post Bureau affordability</t>
+  </si>
+  <si>
+    <t>if Product Type = "STANDARD LOAN" then 20.00 else if Product Type = "SPECIAL LOAN" then 25.00 else null</t>
   </si>
 </sst>
 </file>
@@ -838,7 +831,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +848,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -885,19 +878,19 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>105</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -914,8 +907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,23 +920,23 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
-    <row r="4" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C4" s="23" t="s">
         <v>112</v>
@@ -952,16 +945,16 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -994,44 +987,44 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="D6" s="17"/>
     </row>
@@ -1051,7 +1044,7 @@
   <dimension ref="B2:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1065,12 +1058,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
@@ -1087,31 +1080,31 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1120,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
@@ -1137,14 +1130,14 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>96</v>
+      <c r="F7" s="2">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1152,7 +1145,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
@@ -1169,7 +1162,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>4</v>
@@ -1186,7 +1179,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
@@ -1206,7 +1199,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>4</v>
@@ -1223,7 +1216,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>4</v>
@@ -1243,7 +1236,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="F13" s="2">
         <v>15</v>
@@ -1260,7 +1253,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="F14" s="2">
         <v>18</v>
@@ -1277,7 +1270,7 @@
         <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="F15" s="2">
         <v>45</v>
@@ -1294,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F16" s="2">
         <v>36</v>
@@ -1310,7 +1303,7 @@
   <dimension ref="B1:G10"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1327,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>1</v>
@@ -1354,13 +1347,13 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>13</v>
+        <v>108</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -1378,10 +1371,10 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1429,7 +1422,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
@@ -1441,7 +1434,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1458,10 +1451,10 @@
         <v>4</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -1481,7 +1474,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1494,7 +1487,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,26 +1498,26 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>109</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>25</v>
+        <v>110</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D4" s="17"/>
     </row>
@@ -1533,16 +1526,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D6" s="17"/>
     </row>
@@ -1561,8 +1554,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,12 +1568,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
@@ -1600,16 +1593,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>17</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1620,13 +1613,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1636,10 +1629,10 @@
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1649,10 +1642,10 @@
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="2" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1661,13 +1654,13 @@
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1677,10 +1670,10 @@
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1690,10 +1683,10 @@
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1702,13 +1695,13 @@
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1719,13 +1712,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -1735,10 +1728,10 @@
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1748,10 +1741,10 @@
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="2" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -1760,13 +1753,13 @@
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -1776,10 +1769,10 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1789,10 +1782,10 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1813,7 +1806,7 @@
   <dimension ref="B2:D8"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,62 +1817,62 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D4" s="16"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D6" s="16"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>12</v>
+        <v>109</v>
       </c>
       <c r="D7" s="16"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D8" s="16"/>
     </row>
@@ -1901,7 +1894,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,50 +1906,50 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D6" s="23"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
@@ -1979,7 +1972,7 @@
   <dimension ref="B2:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,26 +1984,26 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="D4" s="16"/>
     </row>
@@ -2028,7 +2021,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2040,12 +2033,12 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
@@ -2059,10 +2052,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2070,7 +2063,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D5" s="2">
         <v>0.6</v>
@@ -2081,7 +2074,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D6" s="2">
         <v>0.7</v>
@@ -2092,7 +2085,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2">
         <v>0.8</v>
@@ -2123,17 +2116,17 @@
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -2141,40 +2134,40 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="8"/>

</xml_diff>

<commit_message>
fixed typo in test data
</commit_message>
<xml_diff>
--- a/test/data/RoutingDecisionService.xlsx
+++ b/test/data/RoutingDecisionService.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670"/>
   </bookViews>
   <sheets>
     <sheet name="Routing" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
   <si>
     <t>service</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>Credit Score</t>
-  </si>
-  <si>
-    <t>Bureau data . Credit Score</t>
   </si>
   <si>
     <t>invocation</t>
@@ -830,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -872,25 +869,25 @@
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D7" s="2"/>
     </row>
@@ -907,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
@@ -920,41 +917,41 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D4" s="23"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>76</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>77</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -987,44 +984,44 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>80</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>81</v>
       </c>
       <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>83</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>84</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>85</v>
       </c>
       <c r="D6" s="17"/>
     </row>
@@ -1058,12 +1055,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
@@ -1080,31 +1077,31 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>90</v>
       </c>
       <c r="F5" s="2"/>
     </row>
@@ -1113,7 +1110,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>4</v>
@@ -1130,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
@@ -1145,7 +1142,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
@@ -1162,7 +1159,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>4</v>
@@ -1179,7 +1176,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>4</v>
@@ -1199,7 +1196,7 @@
         <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>4</v>
@@ -1216,7 +1213,7 @@
         <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>4</v>
@@ -1236,7 +1233,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F13" s="2">
         <v>15</v>
@@ -1253,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F14" s="2">
         <v>18</v>
@@ -1270,7 +1267,7 @@
         <v>4</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F15" s="2">
         <v>45</v>
@@ -1287,7 +1284,7 @@
         <v>4</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" s="2">
         <v>36</v>
@@ -1327,7 +1324,7 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>1</v>
@@ -1347,13 +1344,13 @@
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>8</v>
@@ -1371,10 +1368,10 @@
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
@@ -1422,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>4</v>
@@ -1434,7 +1431,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -1451,10 +1448,10 @@
         <v>4</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -1474,7 +1471,7 @@
         <v>4</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1498,26 +1495,26 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>20</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>21</v>
       </c>
       <c r="D4" s="17"/>
     </row>
@@ -1526,16 +1523,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="17" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>24</v>
       </c>
       <c r="D6" s="17"/>
     </row>
@@ -1568,12 +1565,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
@@ -1593,16 +1590,16 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1613,13 +1610,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1629,10 +1626,10 @@
       <c r="C6" s="18"/>
       <c r="D6" s="18"/>
       <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1642,10 +1639,10 @@
       <c r="C7" s="18"/>
       <c r="D7" s="18"/>
       <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -1654,13 +1651,13 @@
       </c>
       <c r="C8" s="18"/>
       <c r="D8" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1670,10 +1667,10 @@
       <c r="C9" s="18"/>
       <c r="D9" s="18"/>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1683,10 +1680,10 @@
       <c r="C10" s="18"/>
       <c r="D10" s="18"/>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1695,13 +1692,13 @@
       </c>
       <c r="C11" s="18"/>
       <c r="D11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1712,13 +1709,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="F12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -1728,10 +1725,10 @@
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
       <c r="E13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1741,10 +1738,10 @@
       <c r="C14" s="18"/>
       <c r="D14" s="18"/>
       <c r="E14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -1753,13 +1750,13 @@
       </c>
       <c r="C15" s="18"/>
       <c r="D15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="F15" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -1769,10 +1766,10 @@
       <c r="C16" s="18"/>
       <c r="D16" s="18"/>
       <c r="E16" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1782,10 +1779,10 @@
       <c r="C17" s="18"/>
       <c r="D17" s="18"/>
       <c r="E17" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1817,62 +1814,62 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>47</v>
       </c>
       <c r="D4" s="16"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="D5" s="16"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="14" t="s">
         <v>50</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>51</v>
       </c>
       <c r="D6" s="16"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D7" s="16"/>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="14" t="s">
         <v>53</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>54</v>
       </c>
       <c r="D8" s="16"/>
     </row>
@@ -1906,50 +1903,50 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>56</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>57</v>
       </c>
       <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="17"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="23"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="20"/>
       <c r="D7" s="21"/>
@@ -1984,26 +1981,26 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="16"/>
     </row>
@@ -2033,12 +2030,12 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>1</v>
@@ -2052,10 +2049,10 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
@@ -2063,7 +2060,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2">
         <v>0.6</v>
@@ -2074,7 +2071,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2">
         <v>0.7</v>
@@ -2085,7 +2082,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2">
         <v>0.8</v>
@@ -2116,17 +2113,17 @@
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="8"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="17"/>
@@ -2134,40 +2131,40 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>66</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>67</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>68</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>69</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D6" s="17"/>
       <c r="E6" s="8"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>71</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>72</v>
       </c>
       <c r="D7" s="17"/>
       <c r="E7" s="8"/>

</xml_diff>

<commit_message>
- minor change in test data routing decision service - RoutingRules2.xlsx an separate file only capturing the routing rules decision logic - test cases for feel-evaluation - test cases for testing the previously working decision table logic
</commit_message>
<xml_diff>
--- a/test/data/RoutingDecisionService.xlsx
+++ b/test/data/RoutingDecisionService.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670" firstSheet="7" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10905" windowHeight="5670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Routing" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="109">
   <si>
     <t>service</t>
   </si>
@@ -819,7 +819,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D6"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +963,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1032,7 @@
   <dimension ref="B2:F16"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,7 +1120,9 @@
       <c r="C7" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1290,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:G10"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +1477,7 @@
   <dimension ref="B2:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1543,7 +1545,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1882,7 +1884,7 @@
   <dimension ref="B2:D7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+      <selection activeCell="B7" sqref="B7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>